<commit_message>
Added PDF's and Personas
</commit_message>
<xml_diff>
--- a/Xlsx/AcceptanceCriteria.xlsx
+++ b/Xlsx/AcceptanceCriteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemanvithamylapalli/Documents/GitHub/2024S-neon-nomads/Xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA25DD32-4786-E141-8BED-EC82064B9FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8243AD0-B5B4-7E48-A53E-45CCF4B60795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17000" xr2:uid="{577028C0-78C5-4101-B5CB-2623EA44809E}"/>
   </bookViews>
@@ -2659,10 +2659,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4AF4C8-9A46-4932-8C99-CFBA11C0C87F}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2929,5 +2932,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="41" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>